<commit_message>
Updated JSON outputs, added shipsy_code_meenakshi.json, and improved Excel processor
</commit_message>
<xml_diff>
--- a/Shipsy Assignment.xlsx
+++ b/Shipsy Assignment.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <name val="Arial"/>
       <color rgb="FF000000"/>
@@ -68,6 +68,20 @@
       <sz val="10"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color theme="10"/>
+      <sz val="10"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b val="1"/>
     </font>
   </fonts>
@@ -85,7 +99,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -124,16 +138,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -165,9 +195,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -28883,34 +28918,34 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="11" t="inlineStr">
+      <c r="A1" s="14" t="inlineStr">
         <is>
           <t>Company Name</t>
         </is>
       </c>
-      <c r="B1" s="11" t="inlineStr">
+      <c r="B1" s="14" t="inlineStr">
         <is>
           <t>Company Domain</t>
         </is>
       </c>
-      <c r="C1" s="11" t="inlineStr">
+      <c r="C1" s="14" t="inlineStr">
         <is>
           <t>Estimated Revenue (USD)</t>
         </is>
       </c>
-      <c r="D1" s="11" t="inlineStr">
+      <c r="D1" s="14" t="inlineStr">
         <is>
           <t>Tier</t>
         </is>
       </c>
-      <c r="E1" s="11" t="inlineStr">
+      <c r="E1" s="14" t="inlineStr">
         <is>
           <t>Citation</t>
         </is>
@@ -28922,17 +28957,14 @@
           <t>Wincanton</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>1800000000</v>
-      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Super Platinum</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://rocketreach.co/wincanton-profile_b5c6377ff42e0ca3 (Confidence: low) - The only revenue figure found was $1.8 billion in 2025 from RocketReach, which appears to be a business directory rather than an official financial source. The year 2025 suggests this might be a projected or estimated figure rather than actual reported results. No official financial reports or investor relations data was found in the search results.</t>
+          <t>Revenue extraction failed: API call failed after 3 attempts: Rate limit exceeded. Please try again later.</t>
         </is>
       </c>
     </row>
@@ -28949,7 +28981,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (Confidence: low) - No financial information was found for Black Sheep UK in the search results. Without any available data points, official reports, or estimates from credible sources, I cannot determine the company's annual revenue.</t>
+          <t>Revenue extraction failed: API call failed after 3 attempts: Rate limit exceeded. Please try again later.</t>
         </is>
       </c>
     </row>
@@ -28966,7 +28998,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (Confidence: low) - The provided search results only contain contact information (emails and phone numbers) for various Davies Turner employees. There is no financial data, annual reports, or revenue information in any of these results. No authoritative sources like official financial reports or investor relations pages are available in this dataset.</t>
+          <t>Revenue extraction failed: API call failed after 3 attempts: Rate limit exceeded. Please try again later.</t>
         </is>
       </c>
     </row>
@@ -28976,17 +29008,14 @@
           <t>Edrington</t>
         </is>
       </c>
-      <c r="C5" t="n">
-        <v>851100000</v>
-      </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Platinum</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>https://rocketreach.co/edrington-profile_b5c693c4f42e0c9b (Confidence: low) - The only revenue figure found was $851.1 million for 2025 from RocketReach, which appears to be a business directory rather than an official financial report. The 2025 date seems speculative as we're currently in 2024. No official financial statements or investor relations data was found in the search results.</t>
+          <t>Revenue extraction failed: API call failed after 3 attempts: Rate limit exceeded. Please try again later.</t>
         </is>
       </c>
     </row>
@@ -29003,7 +29032,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (Confidence: low) - The search result is for 'Bahrain Middle East Bank' (a banking institution), not 'Bahrain Post' (a postal service). The revenue mentioned (500Kto1M) appears to be for the bank, not the postal service. No relevant information about Bahrain Post's revenue was found in the provided search results.</t>
+          <t>Revenue extraction failed: API call failed after 3 attempts: Rate limit exceeded. Please try again later.</t>
         </is>
       </c>
     </row>
@@ -29020,7 +29049,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (Confidence: low) - The search results explicitly state 'No financial information found for Kuwait Post.' No official financial reports, SEC filings, investor relations pages, or estimates were available in the provided search results to determine annual operating revenue.</t>
+          <t>Revenue extraction failed: API call failed after 3 attempts: Rate limit exceeded. Please try again later.</t>
         </is>
       </c>
     </row>
@@ -29037,7 +29066,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> (Confidence: low) - No financial information was found for Jotun Paints GCC in the search results. Without any available data from official financial reports, SEC filings, investor relations pages, or relevant sources, I cannot determine or estimate the annual revenue.</t>
+          <t>Revenue extraction failed: API call failed after 3 attempts: Rate limit exceeded. Please try again later.</t>
         </is>
       </c>
     </row>
@@ -29047,17 +29076,14 @@
           <t>MAF</t>
         </is>
       </c>
-      <c r="C9" t="n">
-        <v>4100000000</v>
-      </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Super Platinum</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>https://rocketreach.co/maf-dalkia-middle-east-profile_b5cab8e2f42e0bd7 (Confidence: medium) - The search results show multiple companies with 'MAF' in their name across different industries and locations. MAF Dalkia Middle East has the highest reported revenue at $4.1 billion (already in USD) and appears to be the largest entity among the results. Since no specific timeframe is provided for any of the revenue figures, I selected the highest value from what appears to be the most substantial company in the results.</t>
+          <t>Revenue extraction failed: API call failed after 3 attempts: Rate limit exceeded. Please try again later.</t>
         </is>
       </c>
     </row>
@@ -29067,17 +29093,14 @@
           <t>Gulftainer</t>
         </is>
       </c>
-      <c r="C10" t="n">
-        <v>462400000</v>
-      </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Diamond</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>https://rocketreach.co/gulftainer-profile_b5dc5dc1f42e4a6f (Confidence: medium) - The first search result explicitly states Gulftainer's annual revenue was $462.4 million in 2025. While this appears to be a future projection rather than historical data, it's the only revenue figure provided across all search results. The source is a business intelligence platform (RocketReach) rather than an official financial report, which reduces confidence. No conflicting revenue figures were found in other results.</t>
+          <t>Revenue extraction failed: API call failed after 3 attempts: Rate limit exceeded. Please try again later.</t>
         </is>
       </c>
     </row>
@@ -29087,17 +29110,14 @@
           <t>Expeditors</t>
         </is>
       </c>
-      <c r="C11" t="n">
-        <v>8900000000</v>
-      </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Super Platinum</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>https://rocketreach.co/expeditors-international-of-washington-inc-profile_b557e3baf6aeb99e (Confidence: medium) - Multiple RocketReach sources consistently report $8.9 billion in revenue for Expeditors International of Washington Inc. While this is not an official SEC filing or investor relations source, the consistency across multiple entries and the specific mention of the parent company name provides reasonable confidence. However, without access to official financial reports, this should be considered an estimate.</t>
+          <t>Revenue extraction failed: API call failed after 3 attempts: Rate limit exceeded. Please try again later.</t>
         </is>
       </c>
     </row>
@@ -29121,32 +29141,32 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="12" t="inlineStr">
+      <c r="A1" s="14" t="inlineStr">
         <is>
           <t>Contact Name</t>
         </is>
       </c>
-      <c r="B1" s="12" t="inlineStr">
+      <c r="B1" s="14" t="inlineStr">
         <is>
           <t>Company Name</t>
         </is>
       </c>
-      <c r="C1" s="12" t="inlineStr">
+      <c r="C1" s="14" t="inlineStr">
         <is>
           <t>LinkedIn URL</t>
         </is>
       </c>
-      <c r="D1" s="12" t="inlineStr">
+      <c r="D1" s="14" t="inlineStr">
         <is>
           <t>Current Job Title</t>
         </is>
       </c>
-      <c r="E1" s="12" t="inlineStr">
+      <c r="E1" s="14" t="inlineStr">
         <is>
           <t>Work Email</t>
         </is>
       </c>
-      <c r="F1" s="12" t="inlineStr">
+      <c r="F1" s="14" t="inlineStr">
         <is>
           <t>Citation</t>
         </is>
@@ -29165,18 +29185,22 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/juliankelly</t>
+          <t>NOT_FOUND</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Unknown (needs contact agent)</t>
+          <t>NOT_FOUND</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>julian.kelly@about.google</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>LinkedIn Profile</t>
+          <t>Web Search</t>
         </is>
       </c>
     </row>
@@ -29193,18 +29217,22 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/andywong</t>
+          <t>NOT_FOUND</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Unknown (needs contact agent)</t>
+          <t>NOT_FOUND</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>andy.wong@meta.com</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>LinkedIn Profile</t>
+          <t>Web Search</t>
         </is>
       </c>
     </row>
@@ -29221,18 +29249,22 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/anandgupta</t>
+          <t>NOT_FOUND</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Unknown (needs contact agent)</t>
+          <t>NOT_FOUND</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>anand.gupta@adobe.com</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>LinkedIn Profile</t>
+          <t>Web Search</t>
         </is>
       </c>
     </row>
@@ -29249,18 +29281,22 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/sukritihans</t>
+          <t>NOT_FOUND</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Unknown (needs contact agent)</t>
+          <t>NOT_FOUND</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>sukriti.hans@adobe.com</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>LinkedIn Profile</t>
+          <t>Web Search</t>
         </is>
       </c>
     </row>
@@ -29277,18 +29313,22 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/srilakshmiperi</t>
+          <t>NOT_FOUND</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Unknown (needs contact agent)</t>
+          <t>NOT_FOUND</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>srilakshmi.peri@about.google</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>LinkedIn Profile</t>
+          <t>Web Search</t>
         </is>
       </c>
     </row>
@@ -29305,15 +29345,19 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/sriharshabodicherla</t>
+          <t>NOT_FOUND</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Unknown (needs contact agent)</t>
+          <t>NOT_FOUND</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>sriharsha.bodicherla@shipsy.io</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>Web Search</t>
@@ -29333,18 +29377,22 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/parimalas</t>
+          <t>NOT_FOUND</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Unknown (needs contact agent)</t>
+          <t>NOT_FOUND</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>parimala.s@apple.com</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>LinkedIn Profile</t>
+          <t>Web Search</t>
         </is>
       </c>
     </row>
@@ -29361,18 +29409,22 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/saiswarupnerella</t>
+          <t>NOT_FOUND</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Unknown (needs contact agent)</t>
+          <t>NOT_FOUND</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>sai.nerella@hubspot.com</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>LinkedIn Profile</t>
+          <t>Web Search</t>
         </is>
       </c>
     </row>
@@ -29389,15 +29441,19 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/grohithkumar</t>
+          <t>NOT_FOUND</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Unknown (needs contact agent)</t>
+          <t>NOT_FOUND</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>g.kumar@rapidsos.com</t>
+        </is>
+      </c>
       <c r="F10" t="inlineStr">
         <is>
           <t>Web Search</t>
@@ -29417,18 +29473,22 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://www.linkedin.com/in/gaurisaxena</t>
+          <t>NOT_FOUND</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Unknown (needs contact agent)</t>
+          <t>NOT_FOUND</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>gauri.saxena@economictimes.indiatimes.com</t>
+        </is>
+      </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>LinkedIn Profile</t>
+          <t>Web Search</t>
         </is>
       </c>
     </row>

</xml_diff>